<commit_message>
Cleaned up tb octo files so both tanks same line
</commit_message>
<xml_diff>
--- a/Muus Data Log.xlsx
+++ b/Muus Data Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydatrueblood/Desktop/Muusocotpus_leiderma_respiration_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32CFC7E-6095-2E42-AA3E-252B29ED872F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BD0225-4C6C-7E4A-91F5-FC578CC23BC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35460" yWindow="1180" windowWidth="37580" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37580" yWindow="460" windowWidth="37580" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -38,7 +38,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="79">
   <si>
     <t>Date</t>
   </si>
@@ -287,6 +287,12 @@
   </si>
   <si>
     <t>tbocto 1000 rmr tank 3 and 4 day 7 8-18-21-ch1.txt</t>
+  </si>
+  <si>
+    <t>Flow rate 2</t>
+  </si>
+  <si>
+    <t>Mass 2</t>
   </si>
 </sst>
 </file>
@@ -675,18 +681,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD63"/>
+  <dimension ref="A1:AF59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="174" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55:I56"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="174" zoomScaleNormal="174" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:XFD55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="10" max="11" width="14.5" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15.75" customHeight="1">
+    <row r="1" spans="1:32" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,18 +721,22 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="20" t="s">
+      <c r="N1" s="2"/>
+      <c r="O1" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -741,8 +752,10 @@
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
-    </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1">
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+    </row>
+    <row r="2" spans="1:32" ht="15.75" customHeight="1">
       <c r="A2" s="13">
         <v>44389</v>
       </c>
@@ -770,9 +783,11 @@
       <c r="I2" s="16">
         <v>16.8</v>
       </c>
-      <c r="J2" s="4"/>
-    </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1">
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="4"/>
+    </row>
+    <row r="3" spans="1:32" ht="15.75" customHeight="1">
       <c r="A3" s="13">
         <v>44390</v>
       </c>
@@ -800,10 +815,12 @@
       <c r="I3" s="16">
         <v>16.8</v>
       </c>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-    </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1">
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
+    </row>
+    <row r="4" spans="1:32" ht="15.75" customHeight="1">
       <c r="A4" s="20"/>
       <c r="B4" s="20"/>
       <c r="C4" s="4" t="s">
@@ -817,9 +834,9 @@
         <v>0.03</v>
       </c>
       <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-    </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1">
+      <c r="L4" s="20"/>
+    </row>
+    <row r="5" spans="1:32" ht="15.75" customHeight="1">
       <c r="A5" s="8">
         <v>44404</v>
       </c>
@@ -847,11 +864,13 @@
       <c r="I5" s="4">
         <v>20.6</v>
       </c>
-      <c r="K5" s="10">
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="M5" s="10">
         <v>4.9707688000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1">
+    <row r="6" spans="1:32" ht="15.75" customHeight="1">
       <c r="A6" s="8">
         <v>44410</v>
       </c>
@@ -879,11 +898,13 @@
       <c r="I6" s="4">
         <v>2.5</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
         <v>2.1371602300000001</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1">
+    <row r="7" spans="1:32" ht="15.75" customHeight="1">
       <c r="A7" s="8">
         <v>44405</v>
       </c>
@@ -911,12 +932,14 @@
       <c r="I7" s="4">
         <v>2.5</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="4">
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="4">
         <v>4.7088135299999996</v>
       </c>
     </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1">
+    <row r="8" spans="1:32" ht="15.75" customHeight="1">
       <c r="A8" s="8">
         <v>44411</v>
       </c>
@@ -944,15 +967,17 @@
       <c r="I8" s="4">
         <v>2.5</v>
       </c>
-      <c r="J8" s="20"/>
-      <c r="K8" s="12">
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="12">
         <v>14.451878900000001</v>
       </c>
-      <c r="L8" s="7" t="s">
+      <c r="N8" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1">
+    <row r="9" spans="1:32" ht="15.75" customHeight="1">
       <c r="A9" s="8">
         <v>44397</v>
       </c>
@@ -980,12 +1005,14 @@
       <c r="I9" s="4">
         <v>20.6</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4">
         <v>2.3658192200000001</v>
       </c>
-      <c r="K9" s="20"/>
-    </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1">
+      <c r="M9" s="20"/>
+    </row>
+    <row r="10" spans="1:32" ht="15.75" customHeight="1">
       <c r="A10" s="8">
         <v>44403</v>
       </c>
@@ -1013,11 +1040,13 @@
       <c r="I10" s="4">
         <v>20.6</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4">
         <v>2.0620056</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="15.75" customHeight="1">
+    <row r="11" spans="1:32" ht="15.75" customHeight="1">
       <c r="A11" s="8">
         <v>44399</v>
       </c>
@@ -1045,12 +1074,14 @@
       <c r="I11" s="4">
         <v>20.6</v>
       </c>
-      <c r="J11" s="10"/>
-      <c r="K11" s="4">
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="4">
         <v>4.68082976</v>
       </c>
     </row>
-    <row r="12" spans="1:30" ht="15.75" customHeight="1">
+    <row r="12" spans="1:32" ht="15.75" customHeight="1">
       <c r="A12" s="3">
         <v>44389</v>
       </c>
@@ -1078,11 +1109,13 @@
       <c r="I12" s="4">
         <v>30.8</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4">
         <v>2.3543525399999998</v>
       </c>
     </row>
-    <row r="13" spans="1:30" ht="15.75" customHeight="1">
+    <row r="13" spans="1:32" ht="15.75" customHeight="1">
       <c r="A13" s="8">
         <v>44396</v>
       </c>
@@ -1110,13 +1143,15 @@
       <c r="I13" s="4">
         <v>30.8</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4">
         <v>2.70205596</v>
       </c>
-      <c r="K13" s="20"/>
-      <c r="L13" s="20"/>
-    </row>
-    <row r="14" spans="1:30" ht="15.75" customHeight="1">
+      <c r="M13" s="20"/>
+      <c r="N13" s="20"/>
+    </row>
+    <row r="14" spans="1:32" ht="15.75" customHeight="1">
       <c r="A14" s="8">
         <v>44397</v>
       </c>
@@ -1144,12 +1179,14 @@
       <c r="I14" s="4">
         <v>30.8</v>
       </c>
-      <c r="J14" s="20"/>
-      <c r="K14" s="10">
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="20"/>
+      <c r="M14" s="10">
         <v>7.3986612100000002</v>
       </c>
     </row>
-    <row r="15" spans="1:30" ht="15.75" customHeight="1">
+    <row r="15" spans="1:32" ht="15.75" customHeight="1">
       <c r="A15" s="3">
         <v>44390</v>
       </c>
@@ -1177,12 +1214,14 @@
       <c r="I15" s="4">
         <v>30.8</v>
       </c>
-      <c r="J15" s="20"/>
-      <c r="K15" s="4">
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="4">
         <v>5.0152814499999998</v>
       </c>
     </row>
-    <row r="16" spans="1:30" ht="15.75" customHeight="1">
+    <row r="16" spans="1:32" ht="15.75" customHeight="1">
       <c r="A16" s="8">
         <v>44404</v>
       </c>
@@ -1210,12 +1249,14 @@
       <c r="I16" s="4">
         <v>2.5</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4">
         <v>2.6075298899999999</v>
       </c>
-      <c r="K16" s="20"/>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1">
+      <c r="M16" s="20"/>
+    </row>
+    <row r="17" spans="1:15" ht="15.75" customHeight="1">
       <c r="A17" s="8">
         <v>44397</v>
       </c>
@@ -1243,12 +1284,14 @@
       <c r="I17" s="18">
         <v>35</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="20">
         <v>2.4806059899999999</v>
       </c>
-      <c r="K17" s="20"/>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1">
+      <c r="M17" s="20"/>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" customHeight="1">
       <c r="A18" s="8">
         <v>44399</v>
       </c>
@@ -1276,12 +1319,14 @@
       <c r="I18" s="18">
         <v>35</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="21">
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="21">
         <v>3.7745197799999999</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1">
+    <row r="19" spans="1:15" ht="15.75" customHeight="1">
       <c r="A19" s="8">
         <v>44403</v>
       </c>
@@ -1309,11 +1354,13 @@
       <c r="I19" s="18">
         <v>35</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="18"/>
+      <c r="K19" s="18"/>
+      <c r="L19" s="4">
         <v>1.93381425</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1">
+    <row r="20" spans="1:15" ht="15.75" customHeight="1">
       <c r="A20" s="8">
         <v>44404</v>
       </c>
@@ -1341,15 +1388,17 @@
       <c r="I20" s="18">
         <v>35</v>
       </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="22">
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="22">
         <v>10.07637222</v>
       </c>
-      <c r="L20" s="7" t="s">
+      <c r="N20" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="15.75" customHeight="1">
+    <row r="21" spans="1:15" ht="15.75" customHeight="1">
       <c r="A21" s="8">
         <v>44396</v>
       </c>
@@ -1377,11 +1426,13 @@
       <c r="I21" s="18">
         <v>16.8</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="4">
         <v>2.8566023399999998</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="15.75" customHeight="1">
+    <row r="22" spans="1:15" ht="15.75" customHeight="1">
       <c r="A22" s="8">
         <v>44397</v>
       </c>
@@ -1409,13 +1460,15 @@
       <c r="I22" s="18">
         <v>16.8</v>
       </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="21">
+      <c r="J22" s="18"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="19"/>
+      <c r="M22" s="21">
         <v>6.6523577300000003</v>
       </c>
-      <c r="L22" s="5"/>
-    </row>
-    <row r="23" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" customHeight="1">
       <c r="A23" s="8">
         <v>44404</v>
       </c>
@@ -1443,14 +1496,16 @@
       <c r="I23" s="16">
         <v>26</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="4">
         <v>2.0572140000000001</v>
       </c>
-      <c r="M23" t="s">
+      <c r="O23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="15.75" customHeight="1">
+    <row r="24" spans="1:15" ht="15.75" customHeight="1">
       <c r="A24" s="8">
         <v>44410</v>
       </c>
@@ -1478,12 +1533,14 @@
       <c r="I24" s="18">
         <v>26</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="4">
         <v>2.1787546199999999</v>
       </c>
-      <c r="K24" s="20"/>
-    </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1">
+      <c r="M24" s="20"/>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" customHeight="1">
       <c r="A25" s="8">
         <v>44411</v>
       </c>
@@ -1511,12 +1568,14 @@
       <c r="I25" s="16">
         <v>26</v>
       </c>
-      <c r="J25" s="23"/>
-      <c r="L25" s="7" t="s">
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="23"/>
+      <c r="N25" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1">
+    <row r="26" spans="1:15" ht="15.75" customHeight="1">
       <c r="A26" s="8">
         <v>44405</v>
       </c>
@@ -1544,13 +1603,15 @@
       <c r="I26" s="18">
         <v>26</v>
       </c>
-      <c r="J26" s="19"/>
-      <c r="K26" s="21">
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="21">
         <v>5.9150476100000002</v>
       </c>
-      <c r="L26" s="20"/>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N26" s="20"/>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" customHeight="1">
       <c r="A27" s="8">
         <v>44397</v>
       </c>
@@ -1578,14 +1639,16 @@
       <c r="I27" s="4">
         <v>21.6</v>
       </c>
-      <c r="J27" s="5">
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="5">
         <v>2.6881919999999999</v>
       </c>
-      <c r="M27" t="s">
+      <c r="O27" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1">
+    <row r="28" spans="1:15" ht="15.75" customHeight="1">
       <c r="A28" s="8">
         <v>44399</v>
       </c>
@@ -1613,12 +1676,14 @@
       <c r="I28" s="4">
         <v>21.6</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" s="5">
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="5">
         <v>5.1397810000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="15.75" customHeight="1">
+    <row r="29" spans="1:15" ht="15.75" customHeight="1">
       <c r="A29" s="8">
         <v>44403</v>
       </c>
@@ -1646,12 +1711,14 @@
       <c r="I29" s="4">
         <v>21.6</v>
       </c>
-      <c r="J29" s="5">
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="5">
         <v>1.6633500000000001</v>
       </c>
-      <c r="K29" s="20"/>
-    </row>
-    <row r="30" spans="1:13" ht="15.75" customHeight="1">
+      <c r="M29" s="20"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" customHeight="1">
       <c r="A30" s="8">
         <v>44404</v>
       </c>
@@ -1679,11 +1746,13 @@
       <c r="I30" s="4">
         <v>16.899999999999999</v>
       </c>
-      <c r="J30" s="5">
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="5">
         <v>1.94083227</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:15" ht="14">
       <c r="A31" s="8">
         <v>44410</v>
       </c>
@@ -1711,13 +1780,15 @@
       <c r="I31" s="4">
         <v>16.899999999999999</v>
       </c>
-      <c r="J31" s="5">
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="5">
         <v>2.4297590900000001</v>
       </c>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" customHeight="1">
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" customHeight="1">
       <c r="A32" s="3">
         <v>44389</v>
       </c>
@@ -1745,11 +1816,13 @@
       <c r="I32" s="4">
         <v>70</v>
       </c>
-      <c r="J32" s="5">
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="5">
         <v>1.8901110000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1">
+    <row r="33" spans="1:14" ht="15.75" customHeight="1">
       <c r="A33" s="8">
         <v>44397</v>
       </c>
@@ -1777,13 +1850,15 @@
       <c r="I33" s="4">
         <v>70</v>
       </c>
-      <c r="J33" s="20"/>
-      <c r="K33" s="5">
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="5">
         <v>4.3920430000000001</v>
       </c>
-      <c r="L33" s="20"/>
-    </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1">
+      <c r="N33" s="20"/>
+    </row>
+    <row r="34" spans="1:14" ht="15.75" customHeight="1">
       <c r="A34" s="8">
         <v>44396</v>
       </c>
@@ -1811,11 +1886,13 @@
       <c r="I34" s="4">
         <v>70</v>
       </c>
-      <c r="J34" s="5">
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="5">
         <v>2.0054750000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1">
+    <row r="35" spans="1:14" ht="15.75" customHeight="1">
       <c r="A35" s="3">
         <v>44390</v>
       </c>
@@ -1843,15 +1920,17 @@
       <c r="I35" s="4">
         <v>70</v>
       </c>
-      <c r="J35" s="20"/>
-      <c r="K35" s="6">
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="6">
         <v>9.7173850000000002</v>
       </c>
-      <c r="L35" s="7" t="s">
+      <c r="N35" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1">
+    <row r="36" spans="1:14" ht="15.75" customHeight="1">
       <c r="A36" s="8">
         <v>44405</v>
       </c>
@@ -1879,12 +1958,14 @@
       <c r="I36" s="4">
         <v>16.899999999999999</v>
       </c>
-      <c r="J36" s="20"/>
-      <c r="K36" s="5">
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="20"/>
+      <c r="M36" s="5">
         <v>3.22736</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1">
+    <row r="37" spans="1:14" ht="15.75" customHeight="1">
       <c r="A37" s="8">
         <v>44411</v>
       </c>
@@ -1912,15 +1993,17 @@
       <c r="I37" s="4">
         <v>16.899999999999999</v>
       </c>
-      <c r="J37" s="20"/>
-      <c r="K37" s="6">
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="20"/>
+      <c r="M37" s="6">
         <v>9.6436770000000003</v>
       </c>
-      <c r="L37" s="7" t="s">
+      <c r="N37" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1">
+    <row r="38" spans="1:14" ht="15.75" customHeight="1">
       <c r="A38" s="8">
         <v>44404</v>
       </c>
@@ -1948,12 +2031,14 @@
       <c r="I38" s="4">
         <v>21.6</v>
       </c>
-      <c r="J38" s="20"/>
-      <c r="K38" s="5">
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="5">
         <v>3.1428769999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1">
+    <row r="39" spans="1:14" ht="15.75" customHeight="1">
       <c r="A39" s="8">
         <v>44398</v>
       </c>
@@ -1981,13 +2066,15 @@
       <c r="I39" s="4">
         <v>15.5</v>
       </c>
-      <c r="J39" s="10">
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="10">
         <v>2.8575662300000002</v>
       </c>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-    </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M39" s="20"/>
+      <c r="N39" s="20"/>
+    </row>
+    <row r="40" spans="1:14" ht="15.75" customHeight="1">
       <c r="A40" s="8">
         <v>44403</v>
       </c>
@@ -2015,11 +2102,13 @@
       <c r="I40" s="4">
         <v>15.5</v>
       </c>
-      <c r="J40" s="10">
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="10">
         <v>2.2496240099999998</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1">
+    <row r="41" spans="1:14" ht="15.75" customHeight="1">
       <c r="A41" s="8">
         <v>44404</v>
       </c>
@@ -2047,13 +2136,15 @@
       <c r="I41" s="4">
         <v>15.5</v>
       </c>
-      <c r="J41" s="20"/>
-      <c r="K41" s="5">
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="20"/>
+      <c r="M41" s="5">
         <v>4.9864579999999998</v>
       </c>
-      <c r="L41" s="20"/>
-    </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1">
+      <c r="N41" s="20"/>
+    </row>
+    <row r="42" spans="1:14" ht="15.75" customHeight="1">
       <c r="A42" s="8">
         <v>44398</v>
       </c>
@@ -2081,12 +2172,14 @@
       <c r="I42" s="4">
         <v>15.5</v>
       </c>
-      <c r="J42" s="20"/>
-      <c r="K42" s="25">
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="25">
         <v>3.7046770000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1">
+    <row r="43" spans="1:14" ht="15.75" customHeight="1">
       <c r="A43" s="8">
         <v>44403</v>
       </c>
@@ -2114,11 +2207,13 @@
       <c r="I43" s="4">
         <v>41.3</v>
       </c>
-      <c r="J43" s="10">
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="10">
         <v>2.0531238900000002</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1">
+    <row r="44" spans="1:14" ht="15.75" customHeight="1">
       <c r="A44" s="8">
         <v>44396</v>
       </c>
@@ -2146,13 +2241,15 @@
       <c r="I44" s="4">
         <v>27.5</v>
       </c>
-      <c r="J44" s="10">
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="10">
         <v>2.3165354499999999</v>
       </c>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-    </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+    </row>
+    <row r="45" spans="1:14" ht="15.75" customHeight="1">
       <c r="A45" s="8">
         <v>44397</v>
       </c>
@@ -2180,15 +2277,17 @@
       <c r="I45" s="4">
         <v>27.5</v>
       </c>
-      <c r="J45" s="20"/>
-      <c r="K45" s="6">
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="6">
         <v>10.910830000000001</v>
       </c>
-      <c r="L45" s="24" t="s">
+      <c r="N45" s="24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1">
+    <row r="46" spans="1:14" ht="15.75" customHeight="1">
       <c r="A46" s="8">
         <v>44410</v>
       </c>
@@ -2216,12 +2315,14 @@
       <c r="I46" s="4">
         <v>41.3</v>
       </c>
-      <c r="J46" s="10">
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="10">
         <v>2.2072040400000001</v>
       </c>
-      <c r="K46" s="20"/>
-    </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M46" s="20"/>
+    </row>
+    <row r="47" spans="1:14" ht="15.75" customHeight="1">
       <c r="A47" s="8">
         <v>44411</v>
       </c>
@@ -2249,12 +2350,14 @@
       <c r="I47" s="4">
         <v>41.3</v>
       </c>
-      <c r="J47" s="20"/>
-      <c r="K47" s="5">
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="20"/>
+      <c r="M47" s="5">
         <v>4.7029940000000003</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1">
+    <row r="48" spans="1:14" ht="15.75" customHeight="1">
       <c r="A48" s="8">
         <v>44405</v>
       </c>
@@ -2282,12 +2385,14 @@
       <c r="I48" s="4">
         <v>41.3</v>
       </c>
-      <c r="J48" s="20"/>
-      <c r="K48" s="5">
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="20"/>
+      <c r="M48" s="5">
         <v>3.4016920000000002</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="15.75" customHeight="1">
+    <row r="49" spans="1:15" ht="15.75" customHeight="1">
       <c r="A49" s="3">
         <v>44389</v>
       </c>
@@ -2315,12 +2420,14 @@
       <c r="I49" s="4">
         <v>27.5</v>
       </c>
-      <c r="J49" s="10">
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="10">
         <v>1.87584544</v>
       </c>
-      <c r="L49" s="20"/>
-    </row>
-    <row r="50" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N49" s="20"/>
+    </row>
+    <row r="50" spans="1:15" ht="15.75" customHeight="1">
       <c r="A50" s="3">
         <v>44390</v>
       </c>
@@ -2348,12 +2455,14 @@
       <c r="I50" s="4">
         <v>27.5</v>
       </c>
-      <c r="J50" s="20"/>
-      <c r="K50" s="5">
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="5">
         <v>6.1932119999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="15.75" customHeight="1">
+    <row r="51" spans="1:15" ht="15.75" customHeight="1">
       <c r="A51" s="3">
         <v>44418</v>
       </c>
@@ -2381,105 +2490,135 @@
       <c r="I51" s="29">
         <v>36.299999999999997</v>
       </c>
-      <c r="J51" s="20"/>
-      <c r="K51" s="20"/>
-      <c r="M51" s="4" t="s">
+      <c r="J51" s="4">
+        <v>2.6499999999999999E-2</v>
+      </c>
+      <c r="K51" s="29">
+        <v>25.1</v>
+      </c>
+      <c r="L51" s="20"/>
+      <c r="M51" s="20"/>
+      <c r="O51" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A52" s="20"/>
-      <c r="B52" s="20"/>
-      <c r="C52" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D52" s="4">
-        <v>1</v>
-      </c>
-      <c r="E52" s="4" t="s">
+    <row r="52" spans="1:15" s="30" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A52" s="28">
+        <v>44426</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="32" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52" s="29">
+        <v>7</v>
+      </c>
+      <c r="E52" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="29">
+        <v>1</v>
+      </c>
+      <c r="G52" s="29">
+        <v>1000</v>
+      </c>
+      <c r="H52" s="29">
+        <v>0.02</v>
+      </c>
+      <c r="I52" s="29">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="J52" s="29">
+        <v>1.9E-2</v>
+      </c>
+      <c r="K52" s="29">
+        <v>25.1</v>
+      </c>
+      <c r="O52" s="29" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A53" s="20"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D53" s="4">
+        <v>1</v>
+      </c>
+      <c r="E53" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="F52" s="4">
-        <v>2</v>
-      </c>
-      <c r="G52" s="4">
+      <c r="F53" s="4">
+        <v>3</v>
+      </c>
+      <c r="G53" s="4">
         <v>1000</v>
       </c>
-      <c r="H52" s="4">
-        <v>2.6499999999999999E-2</v>
-      </c>
-      <c r="I52" s="29">
-        <v>25.1</v>
-      </c>
-      <c r="J52" s="20"/>
-      <c r="K52" s="20"/>
-      <c r="M52" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" s="30" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A53" s="28">
-        <v>44426</v>
-      </c>
-      <c r="B53" s="29" t="s">
-        <v>56</v>
-      </c>
-      <c r="C53" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="D53" s="29">
+      <c r="H53" s="4">
+        <v>2.7E-2</v>
+      </c>
+      <c r="I53" s="4">
+        <v>13</v>
+      </c>
+      <c r="J53" s="4">
+        <v>2.3E-2</v>
+      </c>
+      <c r="K53" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M53" s="20"/>
+      <c r="O53" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A54" s="20"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" s="4">
         <v>7</v>
       </c>
-      <c r="E53" s="29" t="s">
+      <c r="E54" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F53" s="29">
-        <v>1</v>
-      </c>
-      <c r="G53" s="29">
+      <c r="F54" s="4">
+        <v>3</v>
+      </c>
+      <c r="G54" s="4">
         <v>1000</v>
       </c>
-      <c r="H53" s="29">
-        <v>0.02</v>
-      </c>
-      <c r="I53" s="29">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="M53" s="29" t="s">
+      <c r="H54" s="4">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="I54" s="4">
+        <v>13</v>
+      </c>
+      <c r="J54" s="4">
+        <v>1.9E-2</v>
+      </c>
+      <c r="K54" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M54" s="20"/>
+      <c r="O54" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="30" customFormat="1" ht="15.75" customHeight="1">
-      <c r="C54" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="D54" s="29">
-        <v>7</v>
-      </c>
-      <c r="E54" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="29">
-        <v>2</v>
-      </c>
-      <c r="G54" s="29">
-        <v>1000</v>
-      </c>
-      <c r="H54" s="29">
-        <v>1.9E-2</v>
-      </c>
-      <c r="I54" s="29">
-        <v>25.1</v>
-      </c>
-      <c r="M54" s="29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A55" s="20"/>
-      <c r="B55" s="20"/>
+    <row r="55" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A55" s="3">
+        <v>44420</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>48</v>
+      </c>
       <c r="C55" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D55" s="4">
         <v>1</v>
@@ -2488,193 +2627,76 @@
         <v>51</v>
       </c>
       <c r="F55" s="4">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G55" s="4">
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="H55" s="4">
-        <v>2.7E-2</v>
-      </c>
-      <c r="I55" s="4">
-        <v>13</v>
-      </c>
-      <c r="K55" s="20"/>
-      <c r="M55" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="15.75" customHeight="1">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="I55" s="27">
+        <v>46.1</v>
+      </c>
+      <c r="J55" s="27"/>
+      <c r="K55" s="27"/>
+      <c r="M55" s="20"/>
+      <c r="O55" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="15.75" customHeight="1">
       <c r="A56" s="20"/>
       <c r="B56" s="20"/>
-      <c r="C56" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D56" s="4">
-        <v>1</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F56" s="4">
-        <v>4</v>
-      </c>
-      <c r="G56" s="4">
-        <v>1000</v>
-      </c>
-      <c r="H56" s="4">
-        <v>2.3E-2</v>
-      </c>
-      <c r="I56" s="4">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J56" s="20"/>
-      <c r="M56" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D57" s="4">
-        <v>7</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F57" s="4">
-        <v>3</v>
-      </c>
-      <c r="G57" s="4">
-        <v>1000</v>
-      </c>
-      <c r="H57" s="4">
-        <v>1.6500000000000001E-2</v>
-      </c>
-      <c r="I57" s="4">
-        <v>13</v>
-      </c>
-      <c r="K57" s="20"/>
-      <c r="M57" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="D58" s="4">
-        <v>7</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F58" s="4">
-        <v>4</v>
-      </c>
-      <c r="G58" s="4">
-        <v>1000</v>
-      </c>
-      <c r="H58" s="4">
-        <v>1.9E-2</v>
-      </c>
-      <c r="I58" s="4">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="M58" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A59" s="3">
-        <v>44420</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D59" s="4">
-        <v>1</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F59" s="4">
-        <v>10</v>
-      </c>
-      <c r="G59" s="4">
-        <v>1800</v>
-      </c>
-      <c r="H59" s="4">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="I59" s="27">
-        <v>46.1</v>
-      </c>
-      <c r="K59" s="20"/>
-      <c r="M59" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A60" s="20"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="20"/>
-      <c r="H60" s="20"/>
-      <c r="I60" s="20"/>
-      <c r="K60" s="9"/>
-      <c r="M60" s="20"/>
-    </row>
-    <row r="61" spans="1:13" ht="15.75" customHeight="1">
-      <c r="C61" s="20"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="20"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="20"/>
-      <c r="M61" s="20"/>
-    </row>
-    <row r="62" spans="1:13" ht="15.75" customHeight="1">
-      <c r="C62" s="20"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="20"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="20"/>
-      <c r="K62" s="20"/>
-      <c r="M62" s="20"/>
-    </row>
-    <row r="63" spans="1:13" ht="15.75" customHeight="1">
-      <c r="C63" s="20"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="20"/>
-      <c r="H63" s="20"/>
-      <c r="I63" s="20"/>
-      <c r="K63" s="26"/>
-      <c r="M63" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+      <c r="I56" s="20"/>
+      <c r="M56" s="9"/>
+      <c r="O56" s="20"/>
+    </row>
+    <row r="57" spans="1:15" ht="15.75" customHeight="1">
+      <c r="C57" s="20"/>
+      <c r="D57" s="20"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+      <c r="I57" s="20"/>
+      <c r="O57" s="20"/>
+    </row>
+    <row r="58" spans="1:15" ht="15.75" customHeight="1">
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+      <c r="I58" s="20"/>
+      <c r="M58" s="20"/>
+      <c r="O58" s="20"/>
+    </row>
+    <row r="59" spans="1:15" ht="15.75" customHeight="1">
+      <c r="C59" s="20"/>
+      <c r="D59" s="20"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
+      <c r="M59" s="26"/>
+      <c r="O59" s="20"/>
     </row>
   </sheetData>
-  <sortState ref="A2:AD63">
-    <sortCondition ref="C2:C63"/>
+  <sortState ref="A2:AF59">
+    <sortCondition ref="C2:C59"/>
   </sortState>
-  <conditionalFormatting sqref="J39">
+  <conditionalFormatting sqref="L39">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(J39))&gt;0</formula>
+      <formula>LEN(TRIM(L39))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2nd round of cleaning up file names on Muus data log. Green highlights are fixed,  Yellow are not
</commit_message>
<xml_diff>
--- a/Muus Data Log.xlsx
+++ b/Muus Data Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydatrueblood/Desktop/Muusocotpus_leiderma_respiration_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1BD0225-4C6C-7E4A-91F5-FC578CC23BC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9487A8-E5DA-4041-9CDB-1FE6B0540BB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37580" yWindow="460" windowWidth="37580" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2360" yWindow="1640" windowWidth="37580" windowHeight="18600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -121,9 +121,6 @@
     <t>Gr3 Muus 1000 pcrit 7-22-21.txt</t>
   </si>
   <si>
-    <t>Gr3 Muus1000#2 7day pcrit 7-27-21.txt</t>
-  </si>
-  <si>
     <t>Gr3 Muus 1800#2 pcrit 7-28-21.txt</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>gr2muus1000 pcrit 7-21-21.txt</t>
   </si>
   <si>
-    <t>GR4MUUS18007.12.21MUUS-ch1</t>
-  </si>
-  <si>
     <t>GR4MUUS1800Pcrit-7-13-21</t>
   </si>
   <si>
@@ -205,9 +199,6 @@
     <t>TB</t>
   </si>
   <si>
-    <t>tbocto 1000 rmr tank 1 and 2</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -217,9 +208,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>tbocto 1000 rmr tank 3 and 4</t>
-  </si>
-  <si>
     <t>tbocto 1800 rmr 3-4 blank 8-12-21</t>
   </si>
   <si>
@@ -265,9 +253,6 @@
     <t>gr2muus1800-2 pcrit in 25 ml jar 7-29-21 ch2 is blank.txt</t>
   </si>
   <si>
-    <t>gr3 mnk 7.6.21 muua.txt</t>
-  </si>
-  <si>
     <t>gr3 muus 1800 -2 7-27-21.txt</t>
   </si>
   <si>
@@ -293,6 +278,21 @@
   </si>
   <si>
     <t>Mass 2</t>
+  </si>
+  <si>
+    <t>gr3 mnk 7.6.21 muus.txt</t>
+  </si>
+  <si>
+    <t>gr3 muus 1000-2 7day 7-26-21.txt</t>
+  </si>
+  <si>
+    <t>GR4MUUS1800-7-12-21MUUS-ch1.txt</t>
+  </si>
+  <si>
+    <t>tbocto 1000 rmr tank 3 and 4 8-10-21-ch1.txt</t>
+  </si>
+  <si>
+    <t>tbocto 1000 rmr tank 1 and 2 8-10-21 1 ch 1-2 2 ch3-4.txt</t>
   </si>
 </sst>
 </file>
@@ -351,7 +351,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,6 +400,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -413,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -454,6 +460,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,8 +690,8 @@
   </sheetPr>
   <dimension ref="A1:AF59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="174" zoomScaleNormal="174" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:XFD55"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="174" zoomScaleNormal="174" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -722,10 +729,10 @@
         <v>8</v>
       </c>
       <c r="J1" s="20" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
@@ -735,7 +742,7 @@
       </c>
       <c r="N1" s="2"/>
       <c r="O1" s="20" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -763,7 +770,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="4">
         <v>1</v>
@@ -795,7 +802,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -824,7 +831,7 @@
       <c r="A4" s="20"/>
       <c r="B4" s="20"/>
       <c r="C4" s="4" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D4" s="20"/>
       <c r="E4" s="20"/>
@@ -844,7 +851,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="4">
         <v>7</v>
@@ -878,7 +885,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D6" s="4">
         <v>7</v>
@@ -912,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -947,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="4">
         <v>7</v>
@@ -985,7 +992,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="4">
         <v>1</v>
@@ -1020,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D10" s="4">
         <v>7</v>
@@ -1054,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -1089,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -1123,7 +1130,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="4">
         <v>7</v>
@@ -1159,7 +1166,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" s="4">
         <v>7</v>
@@ -1194,7 +1201,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="4">
         <v>1</v>
@@ -1229,7 +1236,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D16" s="4">
         <v>1</v>
@@ -1264,7 +1271,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D17" s="4">
         <v>1</v>
@@ -1299,7 +1306,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="4">
         <v>1</v>
@@ -1334,7 +1341,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D19" s="4">
         <v>7</v>
@@ -1368,7 +1375,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D20" s="4">
         <v>7</v>
@@ -1406,7 +1413,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="4">
         <v>7</v>
@@ -1440,7 +1447,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="4">
         <v>7</v>
@@ -1476,7 +1483,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
@@ -1502,7 +1509,7 @@
         <v>2.0572140000000001</v>
       </c>
       <c r="O23" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1">
@@ -1513,7 +1520,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D24" s="4">
         <v>7</v>
@@ -1548,7 +1555,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D25" s="4">
         <v>7</v>
@@ -1583,7 +1590,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D26" s="4">
         <v>1</v>
@@ -1645,7 +1652,7 @@
         <v>2.6881919999999999</v>
       </c>
       <c r="O27" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1">
@@ -1691,7 +1698,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D29" s="4">
         <v>7</v>
@@ -1726,7 +1733,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D30" s="4">
         <v>1</v>
@@ -1760,7 +1767,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D31" s="4">
         <v>7</v>
@@ -1938,7 +1945,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D36" s="4">
         <v>1</v>
@@ -1973,7 +1980,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D37" s="4">
         <v>7</v>
@@ -2010,8 +2017,8 @@
       <c r="B38" s="4">
         <v>3</v>
       </c>
-      <c r="C38" s="4" t="s">
-        <v>21</v>
+      <c r="C38" s="34" t="s">
+        <v>75</v>
       </c>
       <c r="D38" s="4">
         <v>7</v>
@@ -2046,7 +2053,7 @@
         <v>4</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D39" s="4">
         <v>1</v>
@@ -2082,7 +2089,7 @@
         <v>4</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D40" s="4">
         <v>7</v>
@@ -2116,7 +2123,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D41" s="4">
         <v>7</v>
@@ -2152,7 +2159,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D42" s="4">
         <v>1</v>
@@ -2187,7 +2194,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D43" s="4">
         <v>1</v>
@@ -2221,7 +2228,7 @@
         <v>4</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D44" s="4">
         <v>7</v>
@@ -2257,7 +2264,7 @@
         <v>4</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D45" s="4">
         <v>7</v>
@@ -2295,7 +2302,7 @@
         <v>4</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D46" s="4">
         <v>7</v>
@@ -2330,7 +2337,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D47" s="4">
         <v>7</v>
@@ -2365,13 +2372,13 @@
         <v>4</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F48" s="4">
         <v>11</v>
@@ -2399,8 +2406,8 @@
       <c r="B49" s="4">
         <v>4</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>38</v>
+      <c r="C49" s="34" t="s">
+        <v>76</v>
       </c>
       <c r="D49" s="4">
         <v>1</v>
@@ -2435,7 +2442,7 @@
         <v>4</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D50" s="4">
         <v>1</v>
@@ -2467,10 +2474,10 @@
         <v>44418</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>78</v>
       </c>
       <c r="D51" s="4">
         <v>1</v>
@@ -2499,7 +2506,7 @@
       <c r="L51" s="20"/>
       <c r="M51" s="20"/>
       <c r="O51" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:15" s="30" customFormat="1" ht="15.75" customHeight="1">
@@ -2507,10 +2514,10 @@
         <v>44426</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D52" s="29">
         <v>7</v>
@@ -2537,20 +2544,20 @@
         <v>25.1</v>
       </c>
       <c r="O52" s="29" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="15.75" customHeight="1">
       <c r="A53" s="20"/>
       <c r="B53" s="20"/>
-      <c r="C53" s="4" t="s">
-        <v>53</v>
+      <c r="C53" s="34" t="s">
+        <v>77</v>
       </c>
       <c r="D53" s="4">
         <v>1</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F53" s="4">
         <v>3</v>
@@ -2572,14 +2579,14 @@
       </c>
       <c r="M53" s="20"/>
       <c r="O53" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="15.75" customHeight="1">
       <c r="A54" s="20"/>
       <c r="B54" s="20"/>
       <c r="C54" s="33" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D54" s="4">
         <v>7</v>
@@ -2607,7 +2614,7 @@
       </c>
       <c r="M54" s="20"/>
       <c r="O54" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="15.75" customHeight="1">
@@ -2615,16 +2622,16 @@
         <v>44420</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55" s="4">
+        <v>1</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D55" s="4">
-        <v>1</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="F55" s="4">
         <v>10</v>
@@ -2642,7 +2649,7 @@
       <c r="K55" s="27"/>
       <c r="M55" s="20"/>
       <c r="O55" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="15.75" customHeight="1">

</xml_diff>

<commit_message>
Fixing filename in Muus Data Log.xlsx
</commit_message>
<xml_diff>
--- a/Muus Data Log.xlsx
+++ b/Muus Data Log.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="96">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -148,6 +148,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">0.5095 for flow</t>
     </r>
@@ -294,6 +295,9 @@
     <t xml:space="preserve">Male</t>
   </si>
   <si>
+    <t xml:space="preserve">tbocto 1000 rmr tank 3 and 4 8-10-21-ch1.txt</t>
+  </si>
+  <si>
     <t xml:space="preserve">rmr</t>
   </si>
   <si>
@@ -379,7 +383,7 @@
     <numFmt numFmtId="169" formatCode="0.0"/>
     <numFmt numFmtId="170" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -417,12 +421,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Monaco"/>
@@ -450,7 +448,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -479,12 +477,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF4CCCC"/>
         <bgColor rgb="FFDEDEDE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF46BDC6"/>
-        <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
     <fill>
@@ -528,7 +520,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -565,7 +557,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -573,7 +565,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -601,15 +593,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -617,7 +609,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -625,15 +617,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -645,11 +633,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -714,7 +702,7 @@
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF4CCCC"/>
       <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF46BDC6"/>
+      <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
@@ -741,11 +729,11 @@
   </sheetPr>
   <dimension ref="A1:AF59"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C55" activeCellId="0" sqref="C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.35"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="14.5"/>
@@ -2522,14 +2510,14 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C55" s="24" t="s">
-        <v>69</v>
+      <c r="C55" s="0" t="s">
+        <v>71</v>
       </c>
       <c r="D55" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F55" s="2" t="n">
         <v>3</v>
@@ -2561,13 +2549,13 @@
         <v>68</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D56" s="2" t="n">
         <v>1</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F56" s="2" t="n">
         <v>10</v>
@@ -2578,22 +2566,22 @@
       <c r="H56" s="2" t="n">
         <v>0.032</v>
       </c>
-      <c r="I56" s="25" t="n">
+      <c r="I56" s="24" t="n">
         <v>46.1</v>
       </c>
       <c r="J56" s="2" t="n">
         <v>0.032</v>
       </c>
-      <c r="K56" s="25" t="n">
+      <c r="K56" s="24" t="n">
         <v>46.1</v>
       </c>
       <c r="O56" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C57" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H57" s="2" t="n">
         <v>0.03</v>
@@ -2604,10 +2592,10 @@
         <v>44426</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D58" s="2" t="n">
         <v>7</v>
@@ -2638,8 +2626,8 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C59" s="26" t="s">
-        <v>77</v>
+      <c r="C59" s="25" t="s">
+        <v>78</v>
       </c>
       <c r="D59" s="2" t="n">
         <v>7</v>
@@ -2697,7 +2685,7 @@
       <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.72265625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.83"/>
   </cols>
@@ -2731,7 +2719,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>11</v>
@@ -2740,19 +2728,19 @@
         <v>12</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>13</v>
@@ -2773,7 +2761,7 @@
       <c r="AF1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="n">
+      <c r="A2" s="26" t="n">
         <v>44769</v>
       </c>
       <c r="B2" s="2" t="n">
@@ -2802,7 +2790,7 @@
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-      <c r="L2" s="28" t="n">
+      <c r="L2" s="27" t="n">
         <v>3.142877</v>
       </c>
       <c r="M2" s="2" t="n">
@@ -2829,7 +2817,7 @@
       <c r="AF2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="n">
+      <c r="A3" s="26" t="n">
         <v>44770</v>
       </c>
       <c r="B3" s="2" t="n">
@@ -2858,14 +2846,14 @@
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="28" t="n">
+      <c r="L3" s="27" t="n">
         <v>3.22736</v>
       </c>
       <c r="M3" s="2" t="n">
         <v>3.923466</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
@@ -2887,7 +2875,7 @@
       <c r="AF3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="n">
+      <c r="A4" s="26" t="n">
         <v>44770</v>
       </c>
       <c r="B4" s="2" t="n">
@@ -2916,7 +2904,7 @@
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="28" t="n">
+      <c r="L4" s="27" t="n">
         <v>3.401692</v>
       </c>
       <c r="M4" s="2" t="n">
@@ -2943,7 +2931,7 @@
       <c r="AF4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="n">
+      <c r="A5" s="26" t="n">
         <v>44763</v>
       </c>
       <c r="B5" s="2" t="n">
@@ -2972,7 +2960,7 @@
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
-      <c r="L5" s="28" t="n">
+      <c r="L5" s="27" t="n">
         <v>3.704677</v>
       </c>
       <c r="M5" s="2" t="n">
@@ -2999,7 +2987,7 @@
       <c r="AF5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="n">
+      <c r="A6" s="26" t="n">
         <v>44764</v>
       </c>
       <c r="B6" s="2" t="n">
@@ -3028,7 +3016,7 @@
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-      <c r="L6" s="29" t="n">
+      <c r="L6" s="28" t="n">
         <v>3.77451978</v>
       </c>
       <c r="M6" s="2" t="n">
@@ -3055,7 +3043,7 @@
       <c r="AF6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="n">
+      <c r="A7" s="26" t="n">
         <v>44762</v>
       </c>
       <c r="B7" s="2" t="n">
@@ -3084,14 +3072,14 @@
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
-      <c r="L7" s="28" t="n">
+      <c r="L7" s="27" t="n">
         <v>4.392043</v>
       </c>
       <c r="M7" s="2" t="n">
         <v>4.392149</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
@@ -3113,7 +3101,7 @@
       <c r="AF7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27" t="n">
+      <c r="A8" s="26" t="n">
         <v>44764</v>
       </c>
       <c r="B8" s="2" t="n">
@@ -3169,7 +3157,7 @@
       <c r="AF8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27" t="n">
+      <c r="A9" s="26" t="n">
         <v>44776</v>
       </c>
       <c r="B9" s="2" t="n">
@@ -3198,7 +3186,7 @@
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
-      <c r="L9" s="28" t="n">
+      <c r="L9" s="27" t="n">
         <v>4.702994</v>
       </c>
       <c r="M9" s="2" t="n">
@@ -3225,7 +3213,7 @@
       <c r="AF9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="n">
+      <c r="A10" s="26" t="n">
         <v>44770</v>
       </c>
       <c r="B10" s="2" t="n">
@@ -3261,7 +3249,7 @@
         <v>4.707</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
@@ -3283,7 +3271,7 @@
       <c r="AF10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="27" t="n">
+      <c r="A11" s="26" t="n">
         <v>44769</v>
       </c>
       <c r="B11" s="2" t="n">
@@ -3312,14 +3300,14 @@
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
-      <c r="L11" s="30" t="n">
+      <c r="L11" s="29" t="n">
         <v>4.9707688</v>
       </c>
       <c r="M11" s="2" t="n">
         <v>4.97</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
@@ -3341,7 +3329,7 @@
       <c r="AF11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27" t="n">
+      <c r="A12" s="26" t="n">
         <v>44769</v>
       </c>
       <c r="B12" s="2" t="n">
@@ -3370,7 +3358,7 @@
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
-      <c r="L12" s="28" t="n">
+      <c r="L12" s="27" t="n">
         <v>4.986458</v>
       </c>
       <c r="M12" s="2" t="n">
@@ -3453,7 +3441,7 @@
       <c r="AF13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="n">
+      <c r="A14" s="26" t="n">
         <v>44764</v>
       </c>
       <c r="B14" s="2" t="n">
@@ -3482,7 +3470,7 @@
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
-      <c r="L14" s="28" t="n">
+      <c r="L14" s="27" t="n">
         <v>5.139781</v>
       </c>
       <c r="M14" s="2" t="n">
@@ -3509,7 +3497,7 @@
       <c r="AF14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27" t="n">
+      <c r="A15" s="26" t="n">
         <v>44770</v>
       </c>
       <c r="B15" s="2" t="n">
@@ -3538,14 +3526,14 @@
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
-      <c r="L15" s="29" t="n">
+      <c r="L15" s="28" t="n">
         <v>5.91504761</v>
       </c>
       <c r="M15" s="2" t="n">
         <v>4</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
@@ -3596,14 +3584,14 @@
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
-      <c r="L16" s="28" t="n">
+      <c r="L16" s="27" t="n">
         <v>6.193212</v>
       </c>
       <c r="M16" s="2" t="n">
         <v>6.556591</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
@@ -3625,7 +3613,7 @@
       <c r="AF16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27" t="n">
+      <c r="A17" s="26" t="n">
         <v>44762</v>
       </c>
       <c r="B17" s="2" t="n">
@@ -3654,10 +3642,10 @@
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="L17" s="29" t="n">
+      <c r="L17" s="28" t="n">
         <v>6.65235773</v>
       </c>
-      <c r="M17" s="28" t="n">
+      <c r="M17" s="27" t="n">
         <v>6.65235</v>
       </c>
       <c r="N17" s="2"/>
@@ -3681,7 +3669,7 @@
       <c r="AF17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27" t="n">
+      <c r="A18" s="26" t="n">
         <v>44762</v>
       </c>
       <c r="B18" s="2" t="n">
@@ -3710,7 +3698,7 @@
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="30" t="n">
+      <c r="L18" s="29" t="n">
         <v>7.39866121</v>
       </c>
       <c r="M18" s="2" t="n">
@@ -3737,7 +3725,7 @@
       <c r="AF18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="27" t="n">
+      <c r="A19" s="26" t="n">
         <v>44776</v>
       </c>
       <c r="B19" s="2" t="n">
@@ -3766,14 +3754,14 @@
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="28" t="n">
+      <c r="L19" s="27" t="n">
         <v>9.643677</v>
       </c>
       <c r="M19" s="2" t="n">
         <v>8.4603</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
@@ -3824,14 +3812,14 @@
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-      <c r="L20" s="28" t="n">
+      <c r="L20" s="27" t="n">
         <v>9.717385</v>
       </c>
       <c r="M20" s="2" t="n">
         <v>9.728477</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
@@ -3853,7 +3841,7 @@
       <c r="AF20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="27" t="n">
+      <c r="A21" s="26" t="n">
         <v>44769</v>
       </c>
       <c r="B21" s="2" t="n">
@@ -3882,14 +3870,14 @@
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="29" t="n">
+      <c r="L21" s="28" t="n">
         <v>10.07637222</v>
       </c>
       <c r="M21" s="2" t="n">
         <v>10.0765</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
@@ -3911,7 +3899,7 @@
       <c r="AF21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="27" t="n">
+      <c r="A22" s="26" t="n">
         <v>44762</v>
       </c>
       <c r="B22" s="2" t="n">
@@ -3940,14 +3928,14 @@
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="28" t="n">
+      <c r="L22" s="27" t="n">
         <v>10.91083</v>
       </c>
       <c r="M22" s="2" t="n">
         <v>6.873062</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -3969,7 +3957,7 @@
       <c r="AF22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="27" t="n">
+      <c r="A23" s="26" t="n">
         <v>44776</v>
       </c>
       <c r="B23" s="2" t="n">
@@ -3998,7 +3986,7 @@
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="30" t="n">
+      <c r="L23" s="29" t="n">
         <v>14.4518789</v>
       </c>
       <c r="M23" s="2" t="n">
@@ -4043,7 +4031,7 @@
         <v>4.589631</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
@@ -4170,7 +4158,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>

</xml_diff>

<commit_message>
Moved two missing pcrits into the TB after session folder, and added final pcrits ot the Muus data log pcrit tab
</commit_message>
<xml_diff>
--- a/Muus Data Log.xlsx
+++ b/Muus Data Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydatrueblood/Desktop/Muusoctopus_leioderma_respiration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F93ECF2-1D92-B140-90D2-28D84C446999}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E59EAF-63D5-E844-9A26-FC4A8DC00649}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12360" yWindow="460" windowWidth="19740" windowHeight="19760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3600" yWindow="460" windowWidth="26020" windowHeight="19780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2749,13 +2749,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A721467D-F9E5-FE47-BCD1-A702924500E2}">
   <dimension ref="A1:AF972"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="F1" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="3" max="3" width="39.83203125" customWidth="1"/>
+    <col min="5" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="8" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32">
@@ -2830,22 +2832,22 @@
     </row>
     <row r="2" spans="1:32" ht="14">
       <c r="A2" s="31">
-        <v>44769</v>
+        <v>44763</v>
       </c>
       <c r="B2" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="D2" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" s="2">
         <v>1000</v>
@@ -2854,15 +2856,15 @@
         <v>15</v>
       </c>
       <c r="I2" s="2">
-        <v>21.6</v>
+        <v>15.5</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="30">
-        <v>3.1428769999999999</v>
+        <v>3.7046770000000002</v>
       </c>
       <c r="M2" s="2">
-        <v>3.1428690000000001</v>
+        <v>3.5967210000000001</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
@@ -2884,15 +2886,15 @@
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:32" ht="14">
+    <row r="3" spans="1:32">
       <c r="A3" s="31">
-        <v>44770</v>
+        <v>44764</v>
       </c>
       <c r="B3" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="D3" s="2">
         <v>1</v>
@@ -2901,28 +2903,26 @@
         <v>14</v>
       </c>
       <c r="F3" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2">
-        <v>1800</v>
+        <v>1000</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I3" s="2">
-        <v>16.899999999999999</v>
+        <v>35</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
-      <c r="L3" s="30">
-        <v>3.22736</v>
+      <c r="L3" s="33">
+        <v>3.7745197799999999</v>
       </c>
       <c r="M3" s="2">
-        <v>3.9234659999999999</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>80</v>
-      </c>
+        <v>3.7746279999999999</v>
+      </c>
+      <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -2942,41 +2942,41 @@
       <c r="AE3" s="2"/>
       <c r="AF3" s="2"/>
     </row>
-    <row r="4" spans="1:32" ht="14">
+    <row r="4" spans="1:32">
       <c r="A4" s="31">
-        <v>44770</v>
+        <v>44764</v>
       </c>
       <c r="B4" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="F4" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="G4" s="2">
-        <v>1800</v>
+        <v>1000</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="2">
-        <v>41.3</v>
+        <v>20.6</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
-      <c r="L4" s="30">
-        <v>3.4016920000000002</v>
+      <c r="L4" s="2">
+        <v>4.68082976</v>
       </c>
       <c r="M4" s="2">
-        <v>3.3552050000000002</v>
+        <v>4.6580000000000004</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
@@ -3000,13 +3000,13 @@
     </row>
     <row r="5" spans="1:32" ht="14">
       <c r="A5" s="31">
-        <v>44763</v>
+        <v>44764</v>
       </c>
       <c r="B5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
@@ -3015,7 +3015,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2">
         <v>1000</v>
@@ -3024,15 +3024,15 @@
         <v>15</v>
       </c>
       <c r="I5" s="2">
-        <v>15.5</v>
+        <v>21.6</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="30">
-        <v>3.7046770000000002</v>
+        <v>5.1397810000000002</v>
       </c>
       <c r="M5" s="2">
-        <v>3.5967210000000001</v>
+        <v>5.0411250000000001</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -3055,14 +3055,14 @@
       <c r="AF5" s="2"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="31">
-        <v>44764</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2</v>
+      <c r="A6" s="29">
+        <v>44418</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="D6" s="2">
         <v>1</v>
@@ -3071,27 +3071,31 @@
         <v>14</v>
       </c>
       <c r="F6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2">
         <v>1000</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>15</v>
+      <c r="H6" s="2">
+        <v>2.6499999999999999E-2</v>
       </c>
       <c r="I6" s="2">
-        <v>35</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="33">
-        <v>3.7745197799999999</v>
-      </c>
+        <v>36.299999999999997</v>
+      </c>
+      <c r="J6" s="2">
+        <v>7.83</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L6" s="2"/>
       <c r="M6" s="2">
-        <v>3.7746279999999999</v>
+        <v>3.7443170000000001</v>
       </c>
       <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
+      <c r="O6" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
@@ -3110,47 +3114,47 @@
       <c r="AE6" s="2"/>
       <c r="AF6" s="2"/>
     </row>
-    <row r="7" spans="1:32" ht="14">
-      <c r="A7" s="31">
-        <v>44762</v>
-      </c>
-      <c r="B7" s="2">
-        <v>3</v>
-      </c>
+    <row r="7" spans="1:32">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="D7" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2">
-        <v>1800</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>15</v>
+        <v>1000</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2.6499999999999999E-2</v>
       </c>
       <c r="I7" s="2">
-        <v>70</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="30">
-        <v>4.3920430000000001</v>
-      </c>
+        <v>25.1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>7.83</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="L7" s="2"/>
       <c r="M7" s="2">
-        <v>4.3921489999999999</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+        <v>7.2601639999999996</v>
+      </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -3169,14 +3173,10 @@
       <c r="AF7" s="2"/>
     </row>
     <row r="8" spans="1:32">
-      <c r="A8" s="31">
-        <v>44764</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -3185,27 +3185,31 @@
         <v>14</v>
       </c>
       <c r="F8" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8" s="2">
         <v>1000</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>15</v>
+      <c r="H8" s="2">
+        <v>2.7E-2</v>
       </c>
       <c r="I8" s="2">
-        <v>20.6</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2">
-        <v>4.68082976</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J8" s="2">
+        <v>7.83</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1.837</v>
+      </c>
+      <c r="L8" s="2"/>
       <c r="M8" s="2">
-        <v>4.6580000000000004</v>
+        <v>4.5088759999999999</v>
       </c>
       <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
+      <c r="O8" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -3224,44 +3228,44 @@
       <c r="AE8" s="2"/>
       <c r="AF8" s="2"/>
     </row>
-    <row r="9" spans="1:32" ht="14">
-      <c r="A9" s="31">
-        <v>44776</v>
-      </c>
-      <c r="B9" s="2">
-        <v>4</v>
-      </c>
+    <row r="9" spans="1:32">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="D9" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="2">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G9" s="2">
-        <v>1800</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>15</v>
+        <v>1000</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2.3E-2</v>
       </c>
       <c r="I9" s="2">
-        <v>41.3</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="30">
-        <v>4.7029940000000003</v>
-      </c>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J9" s="2">
+        <v>7.83</v>
+      </c>
+      <c r="K9" s="2">
+        <v>2.851</v>
+      </c>
+      <c r="L9" s="2"/>
       <c r="M9" s="2">
-        <v>4.4529909999999999</v>
+        <v>3.7815780000000001</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
+      <c r="O9" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -3280,45 +3284,43 @@
       <c r="AE9" s="2"/>
       <c r="AF9" s="2"/>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" ht="14">
       <c r="A10" s="31">
-        <v>44770</v>
+        <v>44769</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F10" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G10" s="2">
-        <v>1800</v>
+        <v>1000</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I10" s="2">
-        <v>2.5</v>
+        <v>21.6</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="2">
-        <v>4.7088135299999996</v>
+      <c r="L10" s="30">
+        <v>3.1428769999999999</v>
       </c>
       <c r="M10" s="2">
-        <v>4.7069999999999999</v>
-      </c>
-      <c r="N10" s="2" t="s">
-        <v>84</v>
-      </c>
+        <v>3.1428690000000001</v>
+      </c>
+      <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -3453,42 +3455,44 @@
       <c r="AF12" s="2"/>
     </row>
     <row r="13" spans="1:32">
-      <c r="A13" s="29">
-        <v>44390</v>
+      <c r="A13" s="31">
+        <v>44769</v>
       </c>
       <c r="B13" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G13" s="2">
-        <v>1800</v>
+        <v>1000</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="2">
-        <v>30.8</v>
+        <v>35</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
-      <c r="L13" s="2">
-        <v>5.0152814499999998</v>
+      <c r="L13" s="33">
+        <v>10.07637222</v>
       </c>
       <c r="M13" s="2">
-        <v>5.0149999999999997</v>
-      </c>
-      <c r="N13" s="2"/>
+        <v>10.076499999999999</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -3508,44 +3512,48 @@
       <c r="AE13" s="2"/>
       <c r="AF13" s="2"/>
     </row>
-    <row r="14" spans="1:32" ht="14">
-      <c r="A14" s="31">
-        <v>44764</v>
-      </c>
-      <c r="B14" s="2">
-        <v>3</v>
+    <row r="14" spans="1:32">
+      <c r="A14" s="29">
+        <v>44426</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
       <c r="D14" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G14" s="2">
         <v>1000</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>15</v>
+      <c r="H14" s="2">
+        <v>0.02</v>
       </c>
       <c r="I14" s="2">
-        <v>21.6</v>
-      </c>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="30">
-        <v>5.1397810000000002</v>
-      </c>
+        <v>36.299999999999997</v>
+      </c>
+      <c r="J14" s="2">
+        <v>7.83</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1.35</v>
+      </c>
+      <c r="L14" s="2"/>
       <c r="M14" s="2">
-        <v>5.0411250000000001</v>
+        <v>15.20444</v>
       </c>
       <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+      <c r="O14" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
@@ -3565,45 +3573,43 @@
       <c r="AF14" s="2"/>
     </row>
     <row r="15" spans="1:32">
-      <c r="A15" s="31">
-        <v>44770</v>
-      </c>
-      <c r="B15" s="2">
-        <v>2</v>
-      </c>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="D15" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G15" s="2">
-        <v>1800</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>15</v>
+        <v>1000</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.9E-2</v>
       </c>
       <c r="I15" s="2">
-        <v>2.6</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="33">
-        <v>5.9150476100000002</v>
-      </c>
+        <v>25.1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>7.83</v>
+      </c>
+      <c r="K15" s="2">
+        <v>2.81</v>
+      </c>
+      <c r="L15" s="2"/>
       <c r="M15" s="2">
-        <v>4</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="O15" s="2"/>
+        <v>6.0251320000000002</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
@@ -3622,46 +3628,44 @@
       <c r="AE15" s="2"/>
       <c r="AF15" s="2"/>
     </row>
-    <row r="16" spans="1:32" ht="14">
-      <c r="A16" s="29">
-        <v>44390</v>
-      </c>
-      <c r="B16" s="2">
-        <v>4</v>
-      </c>
+    <row r="16" spans="1:32">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="D16" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="2">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="G16" s="2">
-        <v>1800</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>15</v>
+        <v>1000</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1.6500000000000001E-2</v>
       </c>
       <c r="I16" s="2">
-        <v>27.5</v>
-      </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="30">
-        <v>6.1932119999999999</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="J16" s="2">
+        <v>7.83</v>
+      </c>
+      <c r="K16" s="2">
+        <v>3.3250000000000002</v>
+      </c>
+      <c r="L16" s="2"/>
       <c r="M16" s="2">
-        <v>6.5565910000000001</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="O16" s="2"/>
+        <v>8.5101650000000006</v>
+      </c>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
@@ -3680,15 +3684,11 @@
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
     </row>
-    <row r="17" spans="1:32" ht="14">
-      <c r="A17" s="31">
-        <v>44762</v>
-      </c>
-      <c r="B17" s="2">
-        <v>2</v>
-      </c>
+    <row r="17" spans="1:32">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="D17" s="2">
         <v>7</v>
@@ -3697,27 +3697,31 @@
         <v>14</v>
       </c>
       <c r="F17" s="2">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G17" s="2">
-        <v>1800</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>15</v>
+        <v>1000</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.9E-2</v>
       </c>
       <c r="I17" s="2">
-        <v>16.8</v>
-      </c>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="33">
-        <v>6.6523577300000003</v>
-      </c>
-      <c r="M17" s="30">
-        <v>6.6523500000000002</v>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J17" s="2">
+        <v>7.83</v>
+      </c>
+      <c r="K17" s="2">
+        <v>5.4409999999999998</v>
+      </c>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2">
+        <v>18.67493</v>
       </c>
       <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
+      <c r="O17" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
@@ -3736,24 +3740,24 @@
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
     </row>
-    <row r="18" spans="1:32">
+    <row r="18" spans="1:32" ht="14">
       <c r="A18" s="31">
-        <v>44762</v>
+        <v>44770</v>
       </c>
       <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2">
         <v>1</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="2">
-        <v>7</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G18" s="2">
         <v>1800</v>
@@ -3762,17 +3766,19 @@
         <v>15</v>
       </c>
       <c r="I18" s="2">
-        <v>30.8</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="32">
-        <v>7.3986612100000002</v>
+      <c r="L18" s="30">
+        <v>3.22736</v>
       </c>
       <c r="M18" s="2">
-        <v>7.3559999999999999</v>
-      </c>
-      <c r="N18" s="2"/>
+        <v>3.9234659999999999</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
@@ -3794,22 +3800,22 @@
     </row>
     <row r="19" spans="1:32" ht="14">
       <c r="A19" s="31">
-        <v>44776</v>
+        <v>44770</v>
       </c>
       <c r="B19" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="D19" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="F19" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G19" s="2">
         <v>1800</v>
@@ -3818,19 +3824,17 @@
         <v>15</v>
       </c>
       <c r="I19" s="2">
-        <v>16.899999999999999</v>
+        <v>41.3</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="30">
-        <v>9.6436770000000003</v>
+        <v>3.4016920000000002</v>
       </c>
       <c r="M19" s="2">
-        <v>8.4603000000000002</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>81</v>
-      </c>
+        <v>3.3552050000000002</v>
+      </c>
+      <c r="N19" s="2"/>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
@@ -3850,15 +3854,15 @@
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
     </row>
-    <row r="20" spans="1:32" ht="14">
-      <c r="A20" s="29">
-        <v>44390</v>
+    <row r="20" spans="1:32">
+      <c r="A20" s="31">
+        <v>44770</v>
       </c>
       <c r="B20" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
       <c r="D20" s="2">
         <v>1</v>
@@ -3867,7 +3871,7 @@
         <v>14</v>
       </c>
       <c r="F20" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G20" s="2">
         <v>1800</v>
@@ -3876,18 +3880,18 @@
         <v>15</v>
       </c>
       <c r="I20" s="2">
-        <v>70</v>
+        <v>2.5</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
-      <c r="L20" s="30">
-        <v>9.7173850000000002</v>
+      <c r="L20" s="2">
+        <v>4.7088135299999996</v>
       </c>
       <c r="M20" s="2">
-        <v>9.7284769999999998</v>
+        <v>4.7069999999999999</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
@@ -3909,44 +3913,42 @@
       <c r="AF20" s="2"/>
     </row>
     <row r="21" spans="1:32">
-      <c r="A21" s="31">
-        <v>44769</v>
+      <c r="A21" s="29">
+        <v>44390</v>
       </c>
       <c r="B21" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="D21" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G21" s="2">
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I21" s="2">
-        <v>35</v>
+        <v>30.8</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
-      <c r="L21" s="33">
-        <v>10.07637222</v>
+      <c r="L21" s="2">
+        <v>5.0152814499999998</v>
       </c>
       <c r="M21" s="2">
-        <v>10.076499999999999</v>
-      </c>
-      <c r="N21" s="2" t="s">
-        <v>85</v>
-      </c>
+        <v>5.0149999999999997</v>
+      </c>
+      <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
@@ -3966,24 +3968,24 @@
       <c r="AE21" s="2"/>
       <c r="AF21" s="2"/>
     </row>
-    <row r="22" spans="1:32" ht="14">
+    <row r="22" spans="1:32">
       <c r="A22" s="31">
-        <v>44762</v>
+        <v>44770</v>
       </c>
       <c r="B22" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G22" s="2">
         <v>1800</v>
@@ -3992,18 +3994,18 @@
         <v>15</v>
       </c>
       <c r="I22" s="2">
-        <v>27.5</v>
+        <v>2.6</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
-      <c r="L22" s="30">
-        <v>10.910830000000001</v>
+      <c r="L22" s="33">
+        <v>5.9150476100000002</v>
       </c>
       <c r="M22" s="2">
-        <v>6.873062</v>
+        <v>4</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -4024,24 +4026,24 @@
       <c r="AE22" s="2"/>
       <c r="AF22" s="2"/>
     </row>
-    <row r="23" spans="1:32">
-      <c r="A23" s="31">
-        <v>44776</v>
+    <row r="23" spans="1:32" ht="14">
+      <c r="A23" s="29">
+        <v>44390</v>
       </c>
       <c r="B23" s="2">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="2">
         <v>1</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="2">
-        <v>7</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F23" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G23" s="2">
         <v>1800</v>
@@ -4050,18 +4052,18 @@
         <v>15</v>
       </c>
       <c r="I23" s="2">
-        <v>2.5</v>
+        <v>27.5</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
-      <c r="L23" s="32">
-        <v>14.451878900000001</v>
+      <c r="L23" s="30">
+        <v>6.1932119999999999</v>
       </c>
       <c r="M23" s="2">
-        <v>15.97024</v>
+        <v>6.5565910000000001</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
@@ -4082,24 +4084,44 @@
       <c r="AE23" s="2"/>
       <c r="AF23" s="2"/>
     </row>
-    <row r="24" spans="1:32">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+    <row r="24" spans="1:32" ht="14">
+      <c r="A24" s="29">
+        <v>44390</v>
+      </c>
+      <c r="B24" s="2">
+        <v>3</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" s="2">
+        <v>1</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="2">
+        <v>10</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1800</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="2">
+        <v>70</v>
+      </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
+      <c r="L24" s="30">
+        <v>9.7173850000000002</v>
+      </c>
       <c r="M24" s="2">
-        <v>4.5896309999999998</v>
+        <v>9.7284769999999998</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
@@ -4122,43 +4144,39 @@
     </row>
     <row r="25" spans="1:32">
       <c r="A25" s="29">
-        <v>44418</v>
+        <v>44420</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>63</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D25" s="2">
         <v>1</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F25" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G25" s="2">
-        <v>1000</v>
+        <v>1800</v>
       </c>
       <c r="H25" s="2">
-        <v>2.6499999999999999E-2</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="I25" s="2">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="J25" s="2">
-        <v>7.83</v>
-      </c>
-      <c r="K25" s="2">
-        <v>1.1000000000000001</v>
-      </c>
+        <v>46.1</v>
+      </c>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
@@ -4178,21 +4196,45 @@
       <c r="AE25" s="2"/>
       <c r="AF25" s="2"/>
     </row>
-    <row r="26" spans="1:32" s="21" customFormat="1">
-      <c r="A26" s="29"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+    <row r="26" spans="1:32" s="21" customFormat="1" ht="14">
+      <c r="A26" s="31">
+        <v>44762</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="2">
+        <v>7</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="2">
+        <v>10</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1800</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="2">
+        <v>70</v>
+      </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+      <c r="L26" s="30">
+        <v>4.3920430000000001</v>
+      </c>
+      <c r="M26" s="2">
+        <v>4.3921489999999999</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
@@ -4212,45 +4254,45 @@
       <c r="AE26" s="2"/>
       <c r="AF26" s="2"/>
     </row>
-    <row r="27" spans="1:32">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+    <row r="27" spans="1:32" ht="14">
+      <c r="A27" s="31">
+        <v>44776</v>
+      </c>
+      <c r="B27" s="2">
+        <v>4</v>
+      </c>
       <c r="C27" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D27" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="F27" s="2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="G27" s="2">
-        <v>1000</v>
-      </c>
-      <c r="H27" s="2">
-        <v>2.6499999999999999E-2</v>
+        <v>1800</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="I27" s="2">
-        <v>25.1</v>
-      </c>
-      <c r="J27" s="2">
-        <v>7.83</v>
-      </c>
-      <c r="K27" s="2">
-        <v>2.4500000000000002</v>
-      </c>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
+        <v>41.3</v>
+      </c>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="30">
+        <v>4.7029940000000003</v>
+      </c>
+      <c r="M27" s="2">
+        <v>4.4529909999999999</v>
+      </c>
       <c r="N27" s="2"/>
-      <c r="O27" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>89</v>
-      </c>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
@@ -4268,20 +4310,42 @@
       <c r="AE27" s="2"/>
       <c r="AF27" s="2"/>
     </row>
-    <row r="28" spans="1:32" s="21" customFormat="1">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+    <row r="28" spans="1:32" s="21" customFormat="1" ht="14">
+      <c r="A28" s="31">
+        <v>44762</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="2">
+        <v>7</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="2">
+        <v>9</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1800</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I28" s="2">
+        <v>16.8</v>
+      </c>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
+      <c r="L28" s="33">
+        <v>6.6523577300000003</v>
+      </c>
+      <c r="M28" s="30">
+        <v>6.6523500000000002</v>
+      </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
@@ -4303,43 +4367,43 @@
       <c r="AF28" s="2"/>
     </row>
     <row r="29" spans="1:32">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="A29" s="31">
+        <v>44762</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1</v>
+      </c>
       <c r="C29" s="2" t="s">
-        <v>95</v>
+        <v>30</v>
       </c>
       <c r="D29" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="F29" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G29" s="2">
-        <v>1000</v>
-      </c>
-      <c r="H29" s="2">
-        <v>2.7E-2</v>
+        <v>1800</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="I29" s="2">
-        <v>13</v>
-      </c>
-      <c r="J29" s="2">
-        <v>7.83</v>
-      </c>
-      <c r="K29" s="2">
-        <v>1.837</v>
-      </c>
-      <c r="L29" s="2"/>
+        <v>30.8</v>
+      </c>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="32">
+        <v>7.3986612100000002</v>
+      </c>
       <c r="M29" s="2">
-        <v>4.5088759999999999</v>
+        <v>7.3559999999999999</v>
       </c>
       <c r="N29" s="2"/>
-      <c r="O29" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="O29" s="2"/>
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
@@ -4358,20 +4422,45 @@
       <c r="AE29" s="2"/>
       <c r="AF29" s="2"/>
     </row>
-    <row r="30" spans="1:32" s="21" customFormat="1">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
+    <row r="30" spans="1:32" s="21" customFormat="1" ht="14">
+      <c r="A30" s="31">
+        <v>44776</v>
+      </c>
+      <c r="B30" s="2">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="2">
+        <v>7</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="2">
+        <v>10</v>
+      </c>
+      <c r="G30" s="2">
+        <v>1800</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I30" s="2">
+        <v>16.899999999999999</v>
+      </c>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="L30" s="30">
+        <v>9.6436770000000003</v>
+      </c>
+      <c r="M30" s="2">
+        <v>8.4603000000000002</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
@@ -4391,44 +4480,46 @@
       <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
     </row>
-    <row r="31" spans="1:32">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+    <row r="31" spans="1:32" ht="14">
+      <c r="A31" s="31">
+        <v>44762</v>
+      </c>
+      <c r="B31" s="2">
+        <v>4</v>
+      </c>
       <c r="C31" s="2" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="D31" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>66</v>
+        <v>14</v>
       </c>
       <c r="F31" s="2">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G31" s="2">
-        <v>1000</v>
-      </c>
-      <c r="H31" s="2">
-        <v>2.3E-2</v>
+        <v>1800</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="I31" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J31" s="2">
-        <v>7.83</v>
-      </c>
-      <c r="K31" s="2">
-        <v>2.851</v>
-      </c>
-      <c r="L31" s="2"/>
+        <v>27.5</v>
+      </c>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="30">
+        <v>10.910830000000001</v>
+      </c>
       <c r="M31" s="2">
-        <v>3.7815780000000001</v>
-      </c>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>6.873062</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
@@ -4448,19 +4539,44 @@
       <c r="AF31" s="2"/>
     </row>
     <row r="32" spans="1:32" s="21" customFormat="1">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
+      <c r="A32" s="31">
+        <v>44776</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="2">
+        <v>7</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="2">
+        <v>8</v>
+      </c>
+      <c r="G32" s="2">
+        <v>1800</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="2">
+        <v>2.5</v>
+      </c>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="N32" s="2"/>
+      <c r="L32" s="32">
+        <v>14.451878900000001</v>
+      </c>
+      <c r="M32" s="2">
+        <v>15.97024</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
@@ -4481,41 +4597,25 @@
       <c r="AF32" s="2"/>
     </row>
     <row r="33" spans="1:32">
-      <c r="A33" s="29">
-        <v>44420</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D33" s="2">
-        <v>1</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F33" s="2">
-        <v>10</v>
-      </c>
-      <c r="G33" s="2">
-        <v>1800</v>
-      </c>
-      <c r="H33" s="2">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="I33" s="2">
-        <v>46.1</v>
-      </c>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="M33" s="2">
+        <v>4.5896309999999998</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="O33" s="2"/>
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
@@ -4535,18 +4635,14 @@
       <c r="AF33" s="2"/>
     </row>
     <row r="34" spans="1:32">
-      <c r="A34" s="2"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="2"/>
-      <c r="C34" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2">
-        <v>0.03</v>
-      </c>
+      <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
@@ -4573,45 +4669,21 @@
       <c r="AF34" s="2"/>
     </row>
     <row r="35" spans="1:32">
-      <c r="A35" s="29">
-        <v>44426</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="2">
-        <v>7</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F35" s="2">
-        <v>1</v>
-      </c>
-      <c r="G35" s="2">
-        <v>1000</v>
-      </c>
-      <c r="H35" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="I35" s="2">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="J35" s="2">
-        <v>7.83</v>
-      </c>
-      <c r="K35" s="2">
-        <v>1.35</v>
-      </c>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
-      <c r="O35" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="O35" s="2"/>
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
@@ -4631,7 +4703,7 @@
       <c r="AF35" s="2"/>
     </row>
     <row r="36" spans="1:32" s="21" customFormat="1">
-      <c r="A36" s="29"/>
+      <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -4643,7 +4715,6 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
       <c r="P36" s="2"/>
@@ -4667,39 +4738,19 @@
     <row r="37" spans="1:32">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
-      <c r="C37" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D37" s="2">
-        <v>7</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F37" s="2">
-        <v>2</v>
-      </c>
-      <c r="G37" s="2">
-        <v>1000</v>
-      </c>
-      <c r="H37" s="2">
-        <v>1.9E-2</v>
-      </c>
-      <c r="I37" s="2">
-        <v>25.1</v>
-      </c>
-      <c r="J37" s="2">
-        <v>7.83</v>
-      </c>
-      <c r="K37" s="2">
-        <v>2.81</v>
-      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
       <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
+      <c r="M37" s="21"/>
       <c r="N37" s="2"/>
-      <c r="O37" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
@@ -4721,12 +4772,16 @@
     <row r="38" spans="1:32" s="21" customFormat="1">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
+      <c r="C38" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="H38" s="2">
+        <v>0.03</v>
+      </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -4753,43 +4808,21 @@
       <c r="AF38" s="2"/>
     </row>
     <row r="39" spans="1:32">
-      <c r="A39" s="2"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D39" s="2">
-        <v>7</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F39" s="2">
-        <v>3</v>
-      </c>
-      <c r="G39" s="2">
-        <v>1000</v>
-      </c>
-      <c r="H39" s="2">
-        <v>1.6500000000000001E-2</v>
-      </c>
-      <c r="I39" s="2">
-        <v>13</v>
-      </c>
-      <c r="J39" s="2">
-        <v>7.83</v>
-      </c>
-      <c r="K39" s="2">
-        <v>3.3250000000000002</v>
-      </c>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
       <c r="L39" s="2"/>
-      <c r="M39" s="2">
-        <v>8.5101650000000006</v>
-      </c>
+      <c r="M39" s="2"/>
       <c r="N39" s="2"/>
-      <c r="O39" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="O39" s="2"/>
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
@@ -4845,41 +4878,19 @@
     <row r="41" spans="1:32">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
-      <c r="C41" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D41" s="2">
-        <v>7</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="2">
-        <v>4</v>
-      </c>
-      <c r="G41" s="2">
-        <v>1000</v>
-      </c>
-      <c r="H41" s="2">
-        <v>1.9E-2</v>
-      </c>
-      <c r="I41" s="2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="J41" s="2">
-        <v>7.83</v>
-      </c>
-      <c r="K41" s="2">
-        <v>5.4409999999999998</v>
-      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
       <c r="L41" s="2"/>
-      <c r="M41" s="2">
-        <v>18.67493</v>
-      </c>
+      <c r="M41" s="2"/>
       <c r="N41" s="2"/>
-      <c r="O41" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="O41" s="2"/>
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
@@ -36553,8 +36564,9 @@
       <c r="AF972" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:AF974">
-    <sortCondition ref="L2:L974"/>
+  <sortState ref="A2:AF972">
+    <sortCondition ref="G2:G972"/>
+    <sortCondition ref="D2:D972"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Evaluated if pcrit runs showed clear break point
</commit_message>
<xml_diff>
--- a/Muus Data Log.xlsx
+++ b/Muus Data Log.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lloydatrueblood/Desktop/Muusoctopus_leioderma_respiration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F1AE4B-970A-D544-9FEB-90761D2256BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB71922A-35B7-194C-AFD6-46C94276F8FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30660" yWindow="80" windowWidth="26020" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30660" yWindow="80" windowWidth="26020" windowHeight="19780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
@@ -91,8 +93,55 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="M14" authorId="0" shapeId="0" xr:uid="{24A5862C-0A4D-324F-9095-EB56E7BDBC72}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>LOST
+	-Tanner Buller</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L50" authorId="0" shapeId="0" xr:uid="{21A25BB9-9959-6B48-8B40-D4A845C8095F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">LOST
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">	-Tanner Buller</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="109">
   <si>
     <t>Date</t>
   </si>
@@ -320,6 +369,105 @@
   </si>
   <si>
     <t>tbocto 1000 pcrit tank 3 and 4 8-11-21-ch1.txt</t>
+  </si>
+  <si>
+    <t>Gr1 Muus 1000#2 pcrit 7-27-21 B.txt</t>
+  </si>
+  <si>
+    <t>Gr1 Muus 1000#2 pcrit 7-27-21.txt</t>
+  </si>
+  <si>
+    <t>Gr1 Muus 1800#2 pcrit 7-28-21.txt</t>
+  </si>
+  <si>
+    <t>Gr2 Muus1000#2 pcrit 7-26-21.txt</t>
+  </si>
+  <si>
+    <t>gr2muus 1000 pcrit 7-21-21.txt</t>
+  </si>
+  <si>
+    <t>gr2muus1000-2 pcrit 7-26-21.txt</t>
+  </si>
+  <si>
+    <t>gr2muus1800-2 pcrit 7-28-21.txt</t>
+  </si>
+  <si>
+    <t>gr2muus1800-2 pcrit day7 8-3-21.txt</t>
+  </si>
+  <si>
+    <t>gr2muus1800-2 pcrit in 25 ml jar 7-29-21 ch2 is blank.txt</t>
+  </si>
+  <si>
+    <t>GR2MUUS18007dayPcrit-7-20-21.txt</t>
+  </si>
+  <si>
+    <t>Gr3 Muus 1000 pcrit 7-21-21.txt</t>
+  </si>
+  <si>
+    <t>gr3 muus 1800 7day Pcrit 7-20-21.txt</t>
+  </si>
+  <si>
+    <t>Gr3 Muus 1800#2 pcrit 07-28-21.txt</t>
+  </si>
+  <si>
+    <t>Gr3 Muus 1800#2 pcrit 08-03-21.txt</t>
+  </si>
+  <si>
+    <t>Gr3 Muus1000#2 7 day pcrit 7-27-21.txt</t>
+  </si>
+  <si>
+    <t>GR4MUUS1000#2Pcrit-7-26-21-ch1.txt</t>
+  </si>
+  <si>
+    <t>GR4MUUS1000Pcrit-7-21-21-ch1.txt</t>
+  </si>
+  <si>
+    <t>GR4MUUS1800-7dayPcrit-7-20-21-ch1.txt</t>
+  </si>
+  <si>
+    <t>GR4MUUS1800#2-7dayPcrit-8-3-21-ch1.txt</t>
+  </si>
+  <si>
+    <t>GR4MUUS1800#2Pcrit-7-28-21-ch1.txt</t>
+  </si>
+  <si>
+    <t>GR4MUUS1800Pcrit-7-13-21-ch1.txt</t>
+  </si>
+  <si>
+    <t>tbocto 1000 pcrit tank 1 and 2 day 7 8-19-21.txt</t>
+  </si>
+  <si>
+    <t>tbocto 1000 pcrit tank 3 and 4 8-11-21-ch3.txt</t>
+  </si>
+  <si>
+    <t>tbocto 1000 pcrit tank 3 and 4 day 7 8-19-21-ch1.txt</t>
+  </si>
+  <si>
+    <t>tbocto 1000 pcrit tank 3 and 4 day 7 8-19-21-ch3.txt</t>
+  </si>
+  <si>
+    <t>Tbocto 1000 pcrti tank 1 and 2 8-11-21.txt</t>
+  </si>
+  <si>
+    <t>File Name</t>
+  </si>
+  <si>
+    <t>Obvious pcrit</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Clearly conform</t>
+  </si>
+  <si>
+    <t>tank 2 confrom</t>
   </si>
 </sst>
 </file>
@@ -492,7 +640,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -717,7 +873,7 @@
   </sheetPr>
   <dimension ref="A1:AF64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
+    <sheetView topLeftCell="A35" zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2695,7 +2851,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L39">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(L39))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2705,6 +2861,331 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACBFEA7E-1B1A-964C-A2B6-DD19ABE7AFAA}">
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="254" zoomScaleNormal="254" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="43.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="21" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>98</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="21"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" s="21"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:C37">
+    <sortCondition ref="B2:B37"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29289722-B951-D545-84B4-EB813479E041}">
   <dimension ref="A1:AF34"/>
   <sheetViews>
@@ -3695,4 +4176,2002 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE743C0B-369F-EF4A-B885-3DD43B07EB15}">
+  <dimension ref="A1:AF66"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="2" width="14.5" style="21"/>
+    <col min="3" max="3" width="29.6640625" style="21" customWidth="1"/>
+    <col min="4" max="16384" width="14.5" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" ht="15.75" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+    </row>
+    <row r="2" spans="1:32" ht="14">
+      <c r="A2" s="3">
+        <v>44390</v>
+      </c>
+      <c r="B2" s="4">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4">
+        <v>10</v>
+      </c>
+      <c r="G2" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="4">
+        <v>70</v>
+      </c>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="M2" s="6">
+        <v>9.7173850000000002</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" ht="14">
+      <c r="A3" s="8">
+        <v>44397</v>
+      </c>
+      <c r="B3" s="4">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="4">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="4">
+        <v>70</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="M3" s="5">
+        <v>4.3920430000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" ht="14">
+      <c r="A4" s="8">
+        <v>44399</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="M4" s="5">
+        <v>5.1397810000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" ht="14">
+      <c r="A5" s="8">
+        <v>44404</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="4">
+        <v>7</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="4">
+        <v>3</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="M5" s="5">
+        <v>3.1428769999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" ht="14">
+      <c r="A6" s="8">
+        <v>44405</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="4">
+        <v>10</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="4">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="M6" s="5">
+        <v>3.22736</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" ht="14">
+      <c r="A7" s="8">
+        <v>44411</v>
+      </c>
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="4">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="4">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="M7" s="6">
+        <v>9.6436770000000003</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" ht="14" customHeight="1">
+      <c r="A8" s="3">
+        <v>44390</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="4">
+        <v>8</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="4">
+        <v>30.8</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="M8" s="4">
+        <v>5.0152814499999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" ht="14" customHeight="1">
+      <c r="A9" s="8">
+        <v>44397</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="4">
+        <v>8</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="4">
+        <v>30.8</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="M9" s="10">
+        <v>7.3986612100000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" ht="14" customHeight="1">
+      <c r="A10" s="8">
+        <v>44399</v>
+      </c>
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1</v>
+      </c>
+      <c r="G10" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="4">
+        <v>4.68082976</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" ht="14" customHeight="1">
+      <c r="A11" s="8">
+        <v>44404</v>
+      </c>
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4">
+        <v>7</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="4">
+        <v>1</v>
+      </c>
+      <c r="G11" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="M11" s="10">
+        <v>4.9707688000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="14" customHeight="1">
+      <c r="A12" s="8">
+        <v>44405</v>
+      </c>
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="4">
+        <v>8</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="M12" s="4">
+        <v>4.7088135299999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="14" customHeight="1">
+      <c r="A13" s="8">
+        <v>44411</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="4">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="4">
+        <v>8</v>
+      </c>
+      <c r="G13" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="M13" s="12">
+        <v>14.451878900000001</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="14" customHeight="1">
+      <c r="A14" s="13">
+        <v>44390</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="4">
+        <v>9</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="16">
+        <v>16.8</v>
+      </c>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+    </row>
+    <row r="15" spans="1:32" ht="15.75" customHeight="1">
+      <c r="A15" s="8">
+        <v>44397</v>
+      </c>
+      <c r="B15" s="4">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="4">
+        <v>7</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="4">
+        <v>9</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="18">
+        <v>16.8</v>
+      </c>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="22">
+        <v>6.6523577300000003</v>
+      </c>
+      <c r="N15" s="5"/>
+    </row>
+    <row r="16" spans="1:32" ht="15.75" customHeight="1">
+      <c r="A16" s="8">
+        <v>44399</v>
+      </c>
+      <c r="B16" s="4">
+        <v>2</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="4">
+        <v>2</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="18">
+        <v>35</v>
+      </c>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="19"/>
+      <c r="M16" s="22">
+        <v>3.7745197799999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A17" s="8">
+        <v>44404</v>
+      </c>
+      <c r="B17" s="4">
+        <v>2</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="4">
+        <v>7</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="4">
+        <v>2</v>
+      </c>
+      <c r="G17" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="18">
+        <v>35</v>
+      </c>
+      <c r="J17" s="18"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="23">
+        <v>10.07637222</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A18" s="8">
+        <v>44405</v>
+      </c>
+      <c r="B18" s="4">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="4">
+        <v>1</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="4">
+        <v>9</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H18" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" s="18">
+        <v>2.6</v>
+      </c>
+      <c r="J18" s="18"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="22">
+        <v>5.9150476100000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A19" s="8">
+        <v>44411</v>
+      </c>
+      <c r="B19" s="4">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="4">
+        <v>7</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="4">
+        <v>9</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="16">
+        <v>2.6</v>
+      </c>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="24"/>
+      <c r="N19" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A20" s="3">
+        <v>44390</v>
+      </c>
+      <c r="B20" s="4">
+        <v>4</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="4">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="4">
+        <v>11</v>
+      </c>
+      <c r="G20" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I20" s="4">
+        <v>27.5</v>
+      </c>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="M20" s="5">
+        <v>6.1932119999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A21" s="8">
+        <v>44397</v>
+      </c>
+      <c r="B21" s="4">
+        <v>4</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="4">
+        <v>7</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="4">
+        <v>11</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="4">
+        <v>27.5</v>
+      </c>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="M21" s="6">
+        <v>10.910830000000001</v>
+      </c>
+      <c r="N21" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A22" s="8">
+        <v>44398</v>
+      </c>
+      <c r="B22" s="4">
+        <v>4</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="4">
+        <v>1</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="4">
+        <v>4</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="4">
+        <v>15.5</v>
+      </c>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="M22" s="26">
+        <v>3.7046770000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A23" s="8">
+        <v>44404</v>
+      </c>
+      <c r="B23" s="4">
+        <v>4</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="4">
+        <v>7</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="4">
+        <v>4</v>
+      </c>
+      <c r="G23" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I23" s="4">
+        <v>15.5</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="M23" s="5">
+        <v>4.9864579999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A24" s="8">
+        <v>44405</v>
+      </c>
+      <c r="B24" s="4">
+        <v>4</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F24" s="4">
+        <v>11</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" s="4">
+        <v>41.3</v>
+      </c>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="M24" s="5">
+        <v>3.4016920000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A25" s="8">
+        <v>44411</v>
+      </c>
+      <c r="B25" s="4">
+        <v>4</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="4">
+        <v>7</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="4">
+        <v>11</v>
+      </c>
+      <c r="G25" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="4">
+        <v>41.3</v>
+      </c>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="M25" s="5">
+        <v>4.7029940000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1">
+      <c r="C26" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="4">
+        <v>1</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I26" s="21">
+        <v>46.1</v>
+      </c>
+      <c r="L26" s="21">
+        <v>3.8715190000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="3">
+        <v>44389</v>
+      </c>
+      <c r="B27" s="4">
+        <v>4</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" s="4">
+        <v>1</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="4">
+        <v>11</v>
+      </c>
+      <c r="G27" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1.6E-2</v>
+      </c>
+      <c r="I27" s="4">
+        <v>27.5</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="10">
+        <v>1.87584544</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A28" s="8">
+        <v>44396</v>
+      </c>
+      <c r="B28" s="4">
+        <v>4</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D28" s="4">
+        <v>7</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="4">
+        <v>11</v>
+      </c>
+      <c r="G28" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H28" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I28" s="4">
+        <v>27.5</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="10">
+        <v>2.3165354499999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A29" s="8">
+        <v>44398</v>
+      </c>
+      <c r="B29" s="4">
+        <v>4</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D29" s="4">
+        <v>1</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="4">
+        <v>4</v>
+      </c>
+      <c r="G29" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H29" s="4">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I29" s="4">
+        <v>15.5</v>
+      </c>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="10">
+        <v>2.8575662300000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A30" s="8">
+        <v>44403</v>
+      </c>
+      <c r="B30" s="4">
+        <v>4</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D30" s="4">
+        <v>7</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="4">
+        <v>4</v>
+      </c>
+      <c r="G30" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H30" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I30" s="4">
+        <v>15.5</v>
+      </c>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="10">
+        <v>2.2496240099999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="14" customHeight="1">
+      <c r="A31" s="8">
+        <v>44403</v>
+      </c>
+      <c r="B31" s="4">
+        <v>4</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="4">
+        <v>1</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="4">
+        <v>11</v>
+      </c>
+      <c r="G31" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H31" s="4">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="I31" s="4">
+        <v>41.3</v>
+      </c>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="10">
+        <v>2.0531238900000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" customHeight="1">
+      <c r="A32" s="8">
+        <v>44410</v>
+      </c>
+      <c r="B32" s="4">
+        <v>4</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D32" s="4">
+        <v>7</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="4">
+        <v>11</v>
+      </c>
+      <c r="G32" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H32" s="4">
+        <v>1.95E-2</v>
+      </c>
+      <c r="I32" s="4">
+        <v>41.3</v>
+      </c>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="10">
+        <v>2.2072040400000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A33" s="3">
+        <v>44418</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="4">
+        <v>1</v>
+      </c>
+      <c r="G33" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H33" s="4">
+        <v>2.6499999999999999E-2</v>
+      </c>
+      <c r="I33" s="4">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="J33" s="4">
+        <v>2.6499999999999999E-2</v>
+      </c>
+      <c r="K33" s="4">
+        <v>25.1</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15.75" customHeight="1">
+      <c r="C34" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="4">
+        <v>3</v>
+      </c>
+      <c r="G34" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H34" s="4">
+        <v>2.7E-2</v>
+      </c>
+      <c r="I34" s="4">
+        <v>13</v>
+      </c>
+      <c r="J34" s="4">
+        <v>2.3E-2</v>
+      </c>
+      <c r="K34" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A35" s="3">
+        <v>44420</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="4">
+        <v>10</v>
+      </c>
+      <c r="G35" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H35" s="4">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="I35" s="28">
+        <v>46.1</v>
+      </c>
+      <c r="J35" s="4">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="K35" s="28">
+        <v>46.1</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A36" s="3">
+        <v>44426</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="4">
+        <v>7</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="4">
+        <v>1</v>
+      </c>
+      <c r="G36" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="I36" s="4">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="J36" s="4">
+        <v>1.9E-2</v>
+      </c>
+      <c r="K36" s="4">
+        <v>25.1</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="15.75" customHeight="1">
+      <c r="C37" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" s="4">
+        <v>7</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="4">
+        <v>3</v>
+      </c>
+      <c r="G37" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H37" s="4">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="I37" s="4">
+        <v>13</v>
+      </c>
+      <c r="J37" s="4">
+        <v>1.9E-2</v>
+      </c>
+      <c r="K37" s="4">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A38" s="3">
+        <v>44389</v>
+      </c>
+      <c r="B38" s="4">
+        <v>3</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="4">
+        <v>10</v>
+      </c>
+      <c r="G38" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H38" s="4">
+        <v>4.7550000000000002E-2</v>
+      </c>
+      <c r="I38" s="4">
+        <v>70</v>
+      </c>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="5">
+        <v>1.8901110000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A39" s="8">
+        <v>44396</v>
+      </c>
+      <c r="B39" s="4">
+        <v>3</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="4">
+        <v>7</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" s="4">
+        <v>10</v>
+      </c>
+      <c r="G39" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H39" s="4">
+        <v>4.1250000000000002E-2</v>
+      </c>
+      <c r="I39" s="4">
+        <v>70</v>
+      </c>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="5">
+        <v>2.0054750000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="13" customHeight="1">
+      <c r="A40" s="8">
+        <v>44397</v>
+      </c>
+      <c r="B40" s="4">
+        <v>3</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" s="4">
+        <v>3</v>
+      </c>
+      <c r="G40" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0.50949999999999995</v>
+      </c>
+      <c r="I40" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="5">
+        <v>2.6881919999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A41" s="8">
+        <v>44403</v>
+      </c>
+      <c r="B41" s="4">
+        <v>3</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" s="4">
+        <v>7</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="4">
+        <v>3</v>
+      </c>
+      <c r="G41" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H41" s="4">
+        <v>2.6499999999999999E-2</v>
+      </c>
+      <c r="I41" s="4">
+        <v>21.6</v>
+      </c>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="5">
+        <v>1.6633500000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="14">
+      <c r="A42" s="8">
+        <v>44404</v>
+      </c>
+      <c r="B42" s="4">
+        <v>3</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" s="4">
+        <v>1</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="4">
+        <v>10</v>
+      </c>
+      <c r="G42" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H42" s="4">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="I42" s="4">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="J42" s="4"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="5">
+        <v>1.94083227</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A43" s="8">
+        <v>44410</v>
+      </c>
+      <c r="B43" s="4">
+        <v>3</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="4">
+        <v>7</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" s="4">
+        <v>10</v>
+      </c>
+      <c r="G43" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H43" s="4">
+        <v>2.0250000000000001E-2</v>
+      </c>
+      <c r="I43" s="4">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="5">
+        <v>2.4297590900000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="14" customHeight="1">
+      <c r="A44" s="3">
+        <v>44389</v>
+      </c>
+      <c r="B44" s="4">
+        <v>1</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="4">
+        <v>1</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="4">
+        <v>8</v>
+      </c>
+      <c r="G44" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H44" s="4">
+        <v>4.9500000000000002E-2</v>
+      </c>
+      <c r="I44" s="4">
+        <v>30.8</v>
+      </c>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4">
+        <v>2.3543525399999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A45" s="8">
+        <v>44396</v>
+      </c>
+      <c r="B45" s="4">
+        <v>1</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="4">
+        <v>7</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" s="4">
+        <v>8</v>
+      </c>
+      <c r="G45" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H45" s="4">
+        <v>4.3099999999999999E-2</v>
+      </c>
+      <c r="I45" s="4">
+        <v>30.8</v>
+      </c>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4">
+        <v>2.70205596</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="14" customHeight="1">
+      <c r="A46" s="8">
+        <v>44397</v>
+      </c>
+      <c r="B46" s="4">
+        <v>1</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="4">
+        <v>1</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="4">
+        <v>1</v>
+      </c>
+      <c r="G46" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H46" s="4">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="I46" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4">
+        <v>2.3658192200000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A47" s="8">
+        <v>44403</v>
+      </c>
+      <c r="B47" s="4">
+        <v>1</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D47" s="4">
+        <v>7</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="4">
+        <v>1</v>
+      </c>
+      <c r="G47" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H47" s="4">
+        <v>3.1E-2</v>
+      </c>
+      <c r="I47" s="4">
+        <v>20.6</v>
+      </c>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4">
+        <v>2.0620056</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="14" customHeight="1">
+      <c r="A48" s="8">
+        <v>44404</v>
+      </c>
+      <c r="B48" s="4">
+        <v>1</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D48" s="4">
+        <v>1</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" s="4">
+        <v>8</v>
+      </c>
+      <c r="G48" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H48" s="4">
+        <v>9.3500000000000007E-3</v>
+      </c>
+      <c r="I48" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4">
+        <v>2.6075298899999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A49" s="8">
+        <v>44410</v>
+      </c>
+      <c r="B49" s="4">
+        <v>1</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" s="4">
+        <v>7</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" s="4">
+        <v>8</v>
+      </c>
+      <c r="G49" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H49" s="4">
+        <v>5.3E-3</v>
+      </c>
+      <c r="I49" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="J49" s="4"/>
+      <c r="K49" s="4"/>
+      <c r="L49" s="4">
+        <v>2.1371602300000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" ht="14" customHeight="1">
+      <c r="A50" s="13">
+        <v>44389</v>
+      </c>
+      <c r="B50" s="4">
+        <v>2</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="4">
+        <v>1</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="4">
+        <v>9</v>
+      </c>
+      <c r="G50" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H50" s="15">
+        <v>0.02</v>
+      </c>
+      <c r="I50" s="16">
+        <v>16.8</v>
+      </c>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
+      <c r="L50" s="4"/>
+    </row>
+    <row r="51" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A51" s="8">
+        <v>44396</v>
+      </c>
+      <c r="B51" s="4">
+        <v>2</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D51" s="4">
+        <v>7</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" s="4">
+        <v>9</v>
+      </c>
+      <c r="G51" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H51" s="15">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I51" s="18">
+        <v>16.8</v>
+      </c>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="4">
+        <v>2.8566023399999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" ht="14" customHeight="1">
+      <c r="A52" s="8">
+        <v>44397</v>
+      </c>
+      <c r="B52" s="4">
+        <v>2</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" s="4">
+        <v>1</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="4">
+        <v>2</v>
+      </c>
+      <c r="G52" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H52" s="15">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="I52" s="18">
+        <v>35</v>
+      </c>
+      <c r="J52" s="18"/>
+      <c r="K52" s="18"/>
+      <c r="L52" s="21">
+        <v>2.4806059899999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" ht="14" customHeight="1">
+      <c r="A53" s="8">
+        <v>44403</v>
+      </c>
+      <c r="B53" s="4">
+        <v>2</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D53" s="4">
+        <v>7</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="4">
+        <v>2</v>
+      </c>
+      <c r="G53" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H53" s="15">
+        <v>2.0199999999999999E-2</v>
+      </c>
+      <c r="I53" s="18">
+        <v>35</v>
+      </c>
+      <c r="J53" s="18"/>
+      <c r="K53" s="18"/>
+      <c r="L53" s="4">
+        <v>1.93381425</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A54" s="8">
+        <v>44404</v>
+      </c>
+      <c r="B54" s="4">
+        <v>2</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D54" s="4">
+        <v>1</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" s="4">
+        <v>9</v>
+      </c>
+      <c r="G54" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H54" s="15">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="I54" s="16">
+        <v>2.6</v>
+      </c>
+      <c r="J54" s="16"/>
+      <c r="K54" s="16"/>
+      <c r="L54" s="4">
+        <v>2.0572140000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A55" s="8">
+        <v>44410</v>
+      </c>
+      <c r="B55" s="4">
+        <v>2</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D55" s="4">
+        <v>7</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" s="4">
+        <v>9</v>
+      </c>
+      <c r="G55" s="4">
+        <v>1800</v>
+      </c>
+      <c r="H55" s="15">
+        <v>4.8500000000000001E-2</v>
+      </c>
+      <c r="I55" s="18">
+        <v>2.6</v>
+      </c>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="4">
+        <v>2.1787546199999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="15.75" customHeight="1">
+      <c r="M56" s="9"/>
+    </row>
+    <row r="57" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="58" spans="1:15" ht="15.75" customHeight="1"/>
+    <row r="59" spans="1:15" ht="15.75" customHeight="1">
+      <c r="M59" s="27"/>
+    </row>
+    <row r="60" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A60" s="3"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="4"/>
+      <c r="O60" s="4"/>
+    </row>
+    <row r="61" spans="1:15" ht="15.75" customHeight="1">
+      <c r="C61" s="30"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="4"/>
+      <c r="O61" s="4"/>
+    </row>
+    <row r="62" spans="1:15" ht="15.75" customHeight="1">
+      <c r="C62" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="H62" s="4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="15.75" customHeight="1">
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="1:15">
+      <c r="A64" s="3"/>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="4"/>
+      <c r="O64" s="4"/>
+    </row>
+    <row r="66" ht="15.75" customHeight="1"/>
+  </sheetData>
+  <sortState ref="A2:AF66">
+    <sortCondition ref="E2:E66"/>
+  </sortState>
+  <conditionalFormatting sqref="L39">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(L39))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>